<commit_message>
Dil_frac and seperate expt ws
</commit_message>
<xml_diff>
--- a/Chl_SIO_pier_forcode.xlsx
+++ b/Chl_SIO_pier_forcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyssia\Desktop\Research_Material_Dr_T\Python_practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C27A6C-107A-4E63-AC0A-8CE780A2AFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A19BF5-5B34-4217-9C00-1E939B1302E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="21 &amp; 22 June 2021" sheetId="3" r:id="rId3"/>
     <sheet name="Dilution_Fraction" sheetId="6" r:id="rId4"/>
     <sheet name="not_working_data" sheetId="4" r:id="rId5"/>
-    <sheet name="working_data" sheetId="5" r:id="rId6"/>
+    <sheet name="working_data_exp1" sheetId="5" r:id="rId6"/>
+    <sheet name="working_data_exp2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="178">
   <si>
     <t>Trilogy Fluorometer, calibrated 23 April 2021</t>
   </si>
@@ -719,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -859,6 +860,7 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -33697,41 +33699,41 @@
     </row>
     <row r="46" spans="1:24" ht="28.5" customHeight="1">
       <c r="A46" s="39"/>
-      <c r="R46" s="80"/>
-      <c r="S46" s="81"/>
-      <c r="T46" s="80"/>
-      <c r="U46" s="81"/>
+      <c r="R46" s="81"/>
+      <c r="S46" s="82"/>
+      <c r="T46" s="81"/>
+      <c r="U46" s="82"/>
     </row>
     <row r="47" spans="1:24" ht="15.5">
       <c r="A47" s="39"/>
-      <c r="R47" s="82"/>
-      <c r="S47" s="81"/>
-      <c r="T47" s="82"/>
-      <c r="U47" s="81"/>
+      <c r="R47" s="83"/>
+      <c r="S47" s="82"/>
+      <c r="T47" s="83"/>
+      <c r="U47" s="82"/>
     </row>
     <row r="48" spans="1:24" ht="15.5">
       <c r="A48" s="39"/>
-      <c r="R48" s="81"/>
-      <c r="S48" s="81"/>
-      <c r="T48" s="81"/>
-      <c r="U48" s="81"/>
+      <c r="R48" s="82"/>
+      <c r="S48" s="82"/>
+      <c r="T48" s="82"/>
+      <c r="U48" s="82"/>
     </row>
     <row r="49" spans="1:21" ht="15.5">
       <c r="A49" s="39"/>
       <c r="G49" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="R49" s="81"/>
-      <c r="S49" s="81"/>
-      <c r="T49" s="81"/>
-      <c r="U49" s="81"/>
+      <c r="R49" s="82"/>
+      <c r="S49" s="82"/>
+      <c r="T49" s="82"/>
+      <c r="U49" s="82"/>
     </row>
     <row r="50" spans="1:21" ht="15.5">
       <c r="A50" s="39"/>
-      <c r="R50" s="81"/>
-      <c r="S50" s="81"/>
-      <c r="T50" s="81"/>
-      <c r="U50" s="81"/>
+      <c r="R50" s="82"/>
+      <c r="S50" s="82"/>
+      <c r="T50" s="82"/>
+      <c r="U50" s="82"/>
     </row>
     <row r="51" spans="1:21" ht="28.5" customHeight="1">
       <c r="A51" s="39"/>
@@ -33748,10 +33750,10 @@
         <v>50</v>
       </c>
       <c r="L51" s="10"/>
-      <c r="R51" s="81"/>
-      <c r="S51" s="81"/>
-      <c r="T51" s="81"/>
-      <c r="U51" s="81"/>
+      <c r="R51" s="82"/>
+      <c r="S51" s="82"/>
+      <c r="T51" s="82"/>
+      <c r="U51" s="82"/>
     </row>
     <row r="52" spans="1:21" ht="15.5">
       <c r="A52" s="39"/>
@@ -33890,7 +33892,7 @@
   </sheetPr>
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
+    <sheetView topLeftCell="H7" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:Q27"/>
     </sheetView>
   </sheetViews>
@@ -42670,7 +42672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC62284-8782-40A2-98D4-94A5D66A26F8}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
@@ -42891,8 +42895,8 @@
   </sheetPr>
   <dimension ref="A1:AC1002"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -56834,8 +56838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B838BAB-43D6-4EC3-9D7F-3DF3470597F4}">
   <dimension ref="A1:R130"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="M93" sqref="M93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -61157,1985 +61161,2182 @@
       </c>
     </row>
     <row r="89" spans="1:18">
-      <c r="A89" t="s">
+      <c r="E89"/>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="E90"/>
+    </row>
+    <row r="91" spans="1:18">
+      <c r="E91"/>
+    </row>
+    <row r="92" spans="1:18">
+      <c r="E92"/>
+    </row>
+    <row r="93" spans="1:18">
+      <c r="E93"/>
+    </row>
+    <row r="94" spans="1:18">
+      <c r="E94"/>
+    </row>
+    <row r="95" spans="1:18">
+      <c r="E95"/>
+    </row>
+    <row r="96" spans="1:18">
+      <c r="E96"/>
+    </row>
+    <row r="97" spans="5:5">
+      <c r="E97"/>
+    </row>
+    <row r="98" spans="5:5">
+      <c r="E98"/>
+    </row>
+    <row r="99" spans="5:5">
+      <c r="E99"/>
+    </row>
+    <row r="100" spans="5:5">
+      <c r="E100"/>
+    </row>
+    <row r="101" spans="5:5">
+      <c r="E101"/>
+    </row>
+    <row r="102" spans="5:5">
+      <c r="E102"/>
+    </row>
+    <row r="103" spans="5:5">
+      <c r="E103"/>
+    </row>
+    <row r="104" spans="5:5">
+      <c r="E104"/>
+    </row>
+    <row r="105" spans="5:5">
+      <c r="E105"/>
+    </row>
+    <row r="106" spans="5:5">
+      <c r="E106"/>
+    </row>
+    <row r="107" spans="5:5">
+      <c r="E107"/>
+    </row>
+    <row r="108" spans="5:5">
+      <c r="E108"/>
+    </row>
+    <row r="109" spans="5:5">
+      <c r="E109"/>
+    </row>
+    <row r="110" spans="5:5">
+      <c r="E110"/>
+    </row>
+    <row r="111" spans="5:5">
+      <c r="E111"/>
+    </row>
+    <row r="112" spans="5:5">
+      <c r="E112"/>
+    </row>
+    <row r="113" spans="5:5">
+      <c r="E113"/>
+    </row>
+    <row r="114" spans="5:5">
+      <c r="E114"/>
+    </row>
+    <row r="115" spans="5:5">
+      <c r="E115"/>
+    </row>
+    <row r="116" spans="5:5">
+      <c r="E116"/>
+    </row>
+    <row r="117" spans="5:5">
+      <c r="E117"/>
+    </row>
+    <row r="118" spans="5:5">
+      <c r="E118"/>
+    </row>
+    <row r="119" spans="5:5">
+      <c r="E119"/>
+    </row>
+    <row r="120" spans="5:5">
+      <c r="E120"/>
+    </row>
+    <row r="121" spans="5:5">
+      <c r="E121"/>
+    </row>
+    <row r="122" spans="5:5">
+      <c r="E122"/>
+    </row>
+    <row r="123" spans="5:5">
+      <c r="E123"/>
+    </row>
+    <row r="124" spans="5:5">
+      <c r="E124"/>
+    </row>
+    <row r="125" spans="5:5">
+      <c r="E125"/>
+    </row>
+    <row r="126" spans="5:5">
+      <c r="E126"/>
+    </row>
+    <row r="127" spans="5:5">
+      <c r="E127"/>
+    </row>
+    <row r="128" spans="5:5">
+      <c r="E128"/>
+    </row>
+    <row r="129" spans="5:5">
+      <c r="E129"/>
+    </row>
+    <row r="130" spans="5:5">
+      <c r="E130"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF76F118-2B29-4A54-ACE7-89610F464ED2}">
+  <dimension ref="A1:R43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetData>
+    <row r="1" spans="1:18" s="80" customFormat="1">
+      <c r="A1" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="80" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="80" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
         <v>177</v>
       </c>
-      <c r="B89">
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C89">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89" s="79">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F89">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="G89">
+      <c r="G2">
         <v>88</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>288</v>
       </c>
-      <c r="J89">
+      <c r="J2">
         <v>800.04</v>
       </c>
-      <c r="K89">
+      <c r="K2">
         <v>296824.40999999997</v>
       </c>
-      <c r="M89">
+      <c r="M2">
         <v>186415.16</v>
       </c>
-      <c r="P89">
+      <c r="P2">
         <v>7</v>
       </c>
-      <c r="Q89">
+      <c r="Q2">
         <v>2.4346288892466101</v>
       </c>
-      <c r="R89">
+      <c r="R2">
         <v>0.48803006209936228</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
-      <c r="A90" t="s">
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>177</v>
       </c>
-      <c r="B90">
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C90">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D90">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E90" s="79">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F90">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="G90">
+      <c r="G3">
         <v>89</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>288</v>
       </c>
-      <c r="J90">
+      <c r="J3">
         <v>800.04</v>
       </c>
-      <c r="K90">
+      <c r="K3">
         <v>229365.73</v>
       </c>
-      <c r="M90">
+      <c r="M3">
         <v>139612.31</v>
       </c>
-      <c r="O90">
+      <c r="O3">
         <v>812.55</v>
       </c>
-      <c r="P90">
+      <c r="P3">
         <v>7</v>
       </c>
-      <c r="Q90">
+      <c r="Q3">
         <v>1.9791482076065599</v>
       </c>
-      <c r="R90">
+      <c r="R3">
         <v>0.20972509829618363</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
-      <c r="A91" t="s">
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
         <v>177</v>
       </c>
-      <c r="B91">
+      <c r="B4">
         <v>100</v>
       </c>
-      <c r="C91">
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="D91">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E91" s="79">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F91">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="G91">
+      <c r="G4">
         <v>90</v>
       </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>288</v>
       </c>
-      <c r="J91">
+      <c r="J4">
         <v>800.04</v>
       </c>
-      <c r="K91">
+      <c r="K4">
         <v>224238.56</v>
       </c>
-      <c r="M91">
+      <c r="M4">
         <v>138209.09</v>
       </c>
-      <c r="O91">
+      <c r="O4">
         <v>785.3</v>
       </c>
-      <c r="P91">
+      <c r="P4">
         <v>7</v>
       </c>
-      <c r="Q91">
+      <c r="Q4">
         <v>1.8970315710737515</v>
       </c>
-      <c r="R91">
+      <c r="R4">
         <v>0.26984173497003322</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
-      <c r="A92" t="s">
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="B92">
+      <c r="B5">
         <v>20</v>
       </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92">
-        <v>1</v>
-      </c>
-      <c r="E92" s="79">
-        <v>1</v>
-      </c>
-      <c r="F92">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="G92">
+      <c r="G5">
         <v>91</v>
       </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>288</v>
       </c>
-      <c r="J92">
+      <c r="J5">
         <v>934.33</v>
       </c>
-      <c r="K92">
+      <c r="K5">
         <v>77189.100000000006</v>
       </c>
-      <c r="M92">
+      <c r="M5">
         <v>49613.42</v>
       </c>
-      <c r="P92">
+      <c r="P5">
         <v>7</v>
       </c>
-      <c r="Q92">
+      <c r="Q5">
         <v>0.61433613568627476</v>
       </c>
-      <c r="R92">
+      <c r="R5">
         <v>0.13726583279705867</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
-      <c r="A93" t="s">
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
         <v>73</v>
       </c>
-      <c r="B93">
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="E93" s="79">
-        <v>1</v>
-      </c>
-      <c r="F93">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="G93">
+      <c r="G6">
         <v>92</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>288</v>
       </c>
-      <c r="J93">
+      <c r="J6">
         <v>934.33</v>
       </c>
-      <c r="K93">
+      <c r="K6">
         <v>84216.34</v>
       </c>
-      <c r="M93">
+      <c r="M6">
         <v>60799.66</v>
       </c>
-      <c r="P93">
+      <c r="P6">
         <v>7</v>
       </c>
-      <c r="Q93">
+      <c r="Q6">
         <v>0.52168115897058809</v>
       </c>
-      <c r="R93">
+      <c r="R6">
         <v>0.39938302364607881</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
-      <c r="A94" t="s">
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B94">
+      <c r="B7">
         <v>20</v>
       </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="E94" s="79">
-        <v>1</v>
-      </c>
-      <c r="F94">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="G94">
+      <c r="G7">
         <v>93</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>288</v>
       </c>
-      <c r="J94">
+      <c r="J7">
         <v>934.33</v>
       </c>
-      <c r="K94">
+      <c r="K7">
         <v>72071.240000000005</v>
       </c>
-      <c r="M94">
+      <c r="M7">
         <v>45238.77</v>
       </c>
-      <c r="P94">
+      <c r="P7">
         <v>7</v>
       </c>
-      <c r="Q94">
+      <c r="Q7">
         <v>0.59777876486519632</v>
       </c>
-      <c r="R94">
+      <c r="R7">
         <v>8.7550901659803532E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
-      <c r="A95" t="s">
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
         <v>76</v>
       </c>
-      <c r="B95">
+      <c r="B8">
         <v>40</v>
       </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95">
-        <v>1</v>
-      </c>
-      <c r="E95" s="79">
-        <v>1</v>
-      </c>
-      <c r="F95">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="G95">
+      <c r="G8">
         <v>94</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>288</v>
       </c>
-      <c r="J95">
+      <c r="J8">
         <v>934.33</v>
       </c>
-      <c r="K95">
+      <c r="K8">
         <v>137597.71</v>
       </c>
-      <c r="M95">
+      <c r="M8">
         <v>87852.68</v>
       </c>
-      <c r="P95">
+      <c r="P8">
         <v>7</v>
       </c>
-      <c r="Q95">
+      <c r="Q8">
         <v>1.1082290445710785</v>
       </c>
-      <c r="R95">
+      <c r="R8">
         <v>0.22266584686225444</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
-      <c r="A96" t="s">
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
         <v>76</v>
       </c>
-      <c r="B96">
+      <c r="B9">
         <v>40</v>
       </c>
-      <c r="C96">
-        <v>1</v>
-      </c>
-      <c r="D96">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="E96" s="79">
-        <v>1</v>
-      </c>
-      <c r="F96">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="G96">
+      <c r="G9">
         <v>95</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>288</v>
       </c>
-      <c r="J96">
+      <c r="J9">
         <v>934.33</v>
       </c>
-      <c r="K96">
+      <c r="K9">
         <v>111682.01</v>
       </c>
-      <c r="M96">
+      <c r="M9">
         <v>95743.15</v>
       </c>
-      <c r="P96">
+      <c r="P9">
         <v>7</v>
       </c>
-      <c r="Q96">
+      <c r="Q9">
         <v>0.35508889208333339</v>
       </c>
-      <c r="R96">
+      <c r="R9">
         <v>1.0953400444583337</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
-      <c r="A97" t="s">
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
         <v>76</v>
       </c>
-      <c r="B97">
+      <c r="B10">
         <v>40</v>
       </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-      <c r="D97">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>3</v>
       </c>
-      <c r="E97" s="79">
-        <v>1</v>
-      </c>
-      <c r="F97">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="G97">
+      <c r="G10">
         <v>96</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>288</v>
       </c>
-      <c r="J97">
+      <c r="J10">
         <v>934.33</v>
       </c>
-      <c r="K97">
+      <c r="K10">
         <v>98520.59</v>
       </c>
-      <c r="M97">
+      <c r="M10">
         <v>66371.78</v>
       </c>
-      <c r="P97">
+      <c r="P10">
         <v>7</v>
       </c>
-      <c r="Q97">
+      <c r="Q10">
         <v>0.71621717768382354</v>
       </c>
-      <c r="R97">
+      <c r="R10">
         <v>0.28925997949950999</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
-      <c r="A98" t="s">
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
         <v>78</v>
       </c>
-      <c r="B98">
+      <c r="B11">
         <v>60</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-      <c r="E98" s="79">
-        <v>1</v>
-      </c>
-      <c r="F98">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="G98">
+      <c r="G11">
         <v>97</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>288</v>
       </c>
-      <c r="J98">
+      <c r="J11">
         <v>934.33</v>
       </c>
-      <c r="K98">
+      <c r="K11">
         <v>213361.89</v>
       </c>
-      <c r="M98">
+      <c r="M11">
         <v>132822.15</v>
       </c>
-      <c r="P98">
+      <c r="P11">
         <v>7</v>
       </c>
-      <c r="Q98">
+      <c r="Q11">
         <v>1.7942793302205891</v>
       </c>
-      <c r="R98">
+      <c r="R11">
         <v>0.21786555715441086</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
-      <c r="A99" t="s">
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B99">
+      <c r="B12">
         <v>60</v>
       </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
-      <c r="D99">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="E99" s="79">
-        <v>1</v>
-      </c>
-      <c r="F99">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>2</v>
       </c>
-      <c r="G99">
+      <c r="G12">
         <v>98</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>288</v>
       </c>
-      <c r="J99">
+      <c r="J12">
         <v>934.33</v>
       </c>
-      <c r="K99">
+      <c r="K12">
         <v>239439.76</v>
       </c>
-      <c r="M99">
+      <c r="M12">
         <v>150009.29</v>
       </c>
-      <c r="P99">
+      <c r="P12">
         <v>7</v>
       </c>
-      <c r="Q99">
+      <c r="Q12">
         <v>1.9923486692769612</v>
       </c>
-      <c r="R99">
+      <c r="R12">
         <v>0.28016706648137235</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
-      <c r="A100" t="s">
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
         <v>78</v>
       </c>
-      <c r="B100">
+      <c r="B13">
         <v>60</v>
       </c>
-      <c r="C100">
-        <v>1</v>
-      </c>
-      <c r="D100">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="E100" s="79">
-        <v>1</v>
-      </c>
-      <c r="F100">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
-      <c r="G100">
+      <c r="G13">
         <v>99</v>
       </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <v>288</v>
       </c>
-      <c r="J100">
+      <c r="J13">
         <v>934.33</v>
       </c>
-      <c r="K100">
+      <c r="K13">
         <v>205350</v>
       </c>
-      <c r="M100">
+      <c r="M13">
         <v>129103.03999999999</v>
       </c>
-      <c r="P100">
+      <c r="P13">
         <v>7</v>
       </c>
-      <c r="Q100">
+      <c r="Q13">
         <v>1.6986439777450983</v>
       </c>
-      <c r="R100">
+      <c r="R13">
         <v>0.25715949238823466</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
-      <c r="A101" t="s">
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
         <v>84</v>
       </c>
-      <c r="B101">
+      <c r="B14">
         <v>80</v>
       </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
-      </c>
-      <c r="E101" s="79">
-        <v>1</v>
-      </c>
-      <c r="F101">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>2</v>
       </c>
-      <c r="G101">
+      <c r="G14">
         <v>100</v>
       </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>288</v>
       </c>
-      <c r="J101">
+      <c r="J14">
         <v>934.33</v>
       </c>
-      <c r="K101">
+      <c r="K14">
         <v>277645.56</v>
       </c>
-      <c r="M101">
+      <c r="M14">
         <v>177426.78</v>
       </c>
-      <c r="P101">
+      <c r="P14">
         <v>7</v>
       </c>
-      <c r="Q101">
+      <c r="Q14">
         <v>2.2326926490441177</v>
       </c>
-      <c r="R101">
+      <c r="R14">
         <v>0.45517521230588276</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
-      <c r="A102" t="s">
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
         <v>84</v>
       </c>
-      <c r="B102">
+      <c r="B15">
         <v>80</v>
       </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-      <c r="D102">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="E102" s="79">
-        <v>1</v>
-      </c>
-      <c r="F102">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>2</v>
       </c>
-      <c r="G102">
+      <c r="G15">
         <v>101</v>
       </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>288</v>
       </c>
-      <c r="J102">
+      <c r="J15">
         <v>934.33</v>
       </c>
-      <c r="K102">
+      <c r="K15">
         <v>275267.03000000003</v>
       </c>
-      <c r="M102">
+      <c r="M15">
         <v>171915.23</v>
       </c>
-      <c r="P102">
+      <c r="P15">
         <v>7</v>
       </c>
-      <c r="Q102">
+      <c r="Q15">
         <v>2.3024906522058832</v>
       </c>
-      <c r="R102">
+      <c r="R15">
         <v>0.30188181960245103</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
-      <c r="A103" t="s">
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
         <v>84</v>
       </c>
-      <c r="B103">
+      <c r="B16">
         <v>80</v>
       </c>
-      <c r="C103">
-        <v>1</v>
-      </c>
-      <c r="D103">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>3</v>
       </c>
-      <c r="E103" s="79">
-        <v>1</v>
-      </c>
-      <c r="F103">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>2</v>
       </c>
-      <c r="G103">
+      <c r="G16">
         <v>102</v>
       </c>
-      <c r="H103">
-        <v>1</v>
-      </c>
-      <c r="I103">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>288</v>
       </c>
-      <c r="J103">
+      <c r="J16">
         <v>934.33</v>
       </c>
-      <c r="K103">
+      <c r="K16">
         <v>328070.43</v>
       </c>
-      <c r="M103">
+      <c r="M16">
         <v>208240.78</v>
       </c>
-      <c r="P103">
+      <c r="P16">
         <v>7</v>
       </c>
-      <c r="Q103">
+      <c r="Q16">
         <v>2.6695872639093139</v>
       </c>
-      <c r="R103">
+      <c r="R16">
         <v>0.48508701910735258</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
-      <c r="A104" t="s">
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
         <v>87</v>
       </c>
-      <c r="B104">
+      <c r="B17">
         <v>100</v>
       </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>1</v>
-      </c>
-      <c r="E104" s="79">
-        <v>1</v>
-      </c>
-      <c r="F104">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>2</v>
       </c>
-      <c r="G104">
+      <c r="G17">
         <v>103</v>
       </c>
-      <c r="H104">
-        <v>1</v>
-      </c>
-      <c r="I104">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>288</v>
       </c>
-      <c r="J104">
+      <c r="J17">
         <v>934.33</v>
       </c>
-      <c r="K104">
+      <c r="K17">
         <v>332757.71000000002</v>
       </c>
-      <c r="M104">
+      <c r="M17">
         <v>244438.06</v>
       </c>
-      <c r="P104">
+      <c r="P17">
         <v>7</v>
       </c>
-      <c r="Q104">
+      <c r="Q17">
         <v>1.9676016143995105</v>
       </c>
-      <c r="R104">
+      <c r="R17">
         <v>1.7354312962171565</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
-      <c r="A105" t="s">
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
         <v>87</v>
       </c>
-      <c r="B105">
+      <c r="B18">
         <v>100</v>
       </c>
-      <c r="C105">
-        <v>1</v>
-      </c>
-      <c r="D105">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="E105" s="79">
-        <v>1</v>
-      </c>
-      <c r="F105">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>2</v>
       </c>
-      <c r="G105">
+      <c r="G18">
         <v>104</v>
       </c>
-      <c r="H105">
-        <v>1</v>
-      </c>
-      <c r="I105">
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>288</v>
       </c>
-      <c r="J105">
+      <c r="J18">
         <v>934.33</v>
       </c>
-      <c r="K105">
+      <c r="K18">
         <v>335466.25</v>
       </c>
-      <c r="M105">
+      <c r="M18">
         <v>248146.26</v>
       </c>
-      <c r="P105">
+      <c r="P18">
         <v>7</v>
       </c>
-      <c r="Q105">
+      <c r="Q18">
         <v>1.9453310027083333</v>
       </c>
-      <c r="R105">
+      <c r="R18">
         <v>1.8138780477416672</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
-      <c r="A106" t="s">
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
         <v>87</v>
       </c>
-      <c r="B106">
+      <c r="B19">
         <v>100</v>
       </c>
-      <c r="C106">
-        <v>1</v>
-      </c>
-      <c r="D106">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>3</v>
       </c>
-      <c r="E106" s="79">
-        <v>1</v>
-      </c>
-      <c r="F106">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
-      <c r="G106">
+      <c r="G19">
         <v>105</v>
       </c>
-      <c r="H106">
-        <v>1</v>
-      </c>
-      <c r="I106">
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <v>288</v>
       </c>
-      <c r="J106">
+      <c r="J19">
         <v>934.33</v>
       </c>
-      <c r="K106">
+      <c r="K19">
         <v>357178.43</v>
       </c>
-      <c r="M106">
+      <c r="M19">
         <v>227249.15</v>
       </c>
-      <c r="P106">
+      <c r="P19">
         <v>7</v>
       </c>
-      <c r="Q106">
+      <c r="Q19">
         <v>2.8945887023529413</v>
       </c>
-      <c r="R106">
+      <c r="R19">
         <v>0.54804654585539214</v>
       </c>
     </row>
-    <row r="107" spans="1:18">
-      <c r="A107" t="s">
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
         <v>89</v>
       </c>
-      <c r="B107">
+      <c r="B20">
         <v>100</v>
       </c>
-      <c r="C107">
+      <c r="C20">
         <v>0</v>
       </c>
-      <c r="D107">
-        <v>1</v>
-      </c>
-      <c r="E107" s="79">
-        <v>1</v>
-      </c>
-      <c r="F107">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>2</v>
       </c>
-      <c r="G107">
+      <c r="G20">
         <v>106</v>
       </c>
-      <c r="H107">
-        <v>1</v>
-      </c>
-      <c r="I107">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>288</v>
       </c>
-      <c r="J107">
+      <c r="J20">
         <v>934.33</v>
       </c>
-      <c r="K107">
+      <c r="K20">
         <v>338253.87</v>
       </c>
-      <c r="M107">
+      <c r="M20">
         <v>214920.04</v>
       </c>
-      <c r="P107">
+      <c r="P20">
         <v>7</v>
       </c>
-      <c r="Q107">
+      <c r="Q20">
         <v>2.7476540386887254</v>
       </c>
-      <c r="R107">
+      <c r="R20">
         <v>0.50820546727794202</v>
       </c>
     </row>
-    <row r="108" spans="1:18">
-      <c r="A108" t="s">
+    <row r="21" spans="1:18">
+      <c r="A21" t="s">
         <v>89</v>
       </c>
-      <c r="B108">
+      <c r="B21">
         <v>100</v>
       </c>
-      <c r="C108">
+      <c r="C21">
         <v>0</v>
       </c>
-      <c r="D108">
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="E108" s="79">
-        <v>1</v>
-      </c>
-      <c r="F108">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>2</v>
       </c>
-      <c r="G108">
+      <c r="G21">
         <v>107</v>
       </c>
-      <c r="H108">
-        <v>1</v>
-      </c>
-      <c r="I108">
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>288</v>
       </c>
-      <c r="J108">
+      <c r="J21">
         <v>934.33</v>
       </c>
-      <c r="K108">
+      <c r="K21">
         <v>303494.15000000002</v>
       </c>
-      <c r="M108">
+      <c r="M21">
         <v>193276.93</v>
       </c>
-      <c r="P108">
+      <c r="P21">
         <v>7</v>
       </c>
-      <c r="Q108">
+      <c r="Q21">
         <v>2.4554397578186284</v>
       </c>
-      <c r="R108">
+      <c r="R21">
         <v>0.47254466757303853</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
-      <c r="A109" t="s">
+    <row r="22" spans="1:18">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-      <c r="B109">
+      <c r="B22">
         <v>100</v>
       </c>
-      <c r="C109">
+      <c r="C22">
         <v>0</v>
       </c>
-      <c r="D109">
+      <c r="D22">
         <v>3</v>
       </c>
-      <c r="E109" s="79">
-        <v>1</v>
-      </c>
-      <c r="F109">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>2</v>
       </c>
-      <c r="G109">
+      <c r="G22">
         <v>108</v>
       </c>
-      <c r="H109">
-        <v>1</v>
-      </c>
-      <c r="I109">
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <v>288</v>
       </c>
-      <c r="J109">
+      <c r="J22">
         <v>934.33</v>
       </c>
-      <c r="K109">
+      <c r="K22">
         <v>446538.03</v>
       </c>
-      <c r="M109">
+      <c r="M22">
         <v>293755.25</v>
       </c>
-      <c r="P109">
+      <c r="P22">
         <v>7</v>
       </c>
-      <c r="Q109">
+      <c r="Q22">
         <v>3.4037232323774518</v>
       </c>
-      <c r="R109">
+      <c r="R22">
         <v>1.0464240090808821</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
-      <c r="A110" t="s">
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
         <v>75</v>
       </c>
-      <c r="B110">
+      <c r="B23">
         <v>20</v>
       </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110">
-        <v>1</v>
-      </c>
-      <c r="E110" s="79">
-        <v>1</v>
-      </c>
-      <c r="F110">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>2</v>
       </c>
-      <c r="G110">
+      <c r="G23">
         <v>112</v>
       </c>
-      <c r="H110">
-        <v>1</v>
-      </c>
-      <c r="I110">
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <v>288</v>
       </c>
-      <c r="J110">
+      <c r="J23">
         <v>934.33</v>
       </c>
-      <c r="K110">
+      <c r="K23">
         <v>78697.87</v>
       </c>
-      <c r="M110">
+      <c r="M23">
         <v>50118.98</v>
       </c>
-      <c r="P110">
+      <c r="P23">
         <v>7</v>
       </c>
-      <c r="Q110">
+      <c r="Q23">
         <v>0.63668583493872533</v>
       </c>
-      <c r="R110">
+      <c r="R23">
         <v>0.12257494624460805</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
-      <c r="A111" t="s">
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="B111">
+      <c r="B24">
         <v>20</v>
       </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
-      <c r="D111">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
         <v>2</v>
       </c>
-      <c r="E111" s="79">
-        <v>1</v>
-      </c>
-      <c r="F111">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>2</v>
       </c>
-      <c r="G111">
+      <c r="G24">
         <v>113</v>
       </c>
-      <c r="H111">
-        <v>1</v>
-      </c>
-      <c r="I111">
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <v>288</v>
       </c>
-      <c r="J111">
+      <c r="J24">
         <v>934.33</v>
       </c>
-      <c r="K111">
+      <c r="K24">
         <v>69641.789999999994</v>
       </c>
-      <c r="M111">
+      <c r="M24">
         <v>44154.03</v>
       </c>
-      <c r="P111">
+      <c r="P24">
         <v>7</v>
       </c>
-      <c r="Q111">
+      <c r="Q24">
         <v>0.56782106499999996</v>
       </c>
-      <c r="R111">
+      <c r="R24">
         <v>0.10107569447500003</v>
       </c>
     </row>
-    <row r="112" spans="1:18">
-      <c r="A112" t="s">
+    <row r="25" spans="1:18">
+      <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B112">
+      <c r="B25">
         <v>20</v>
       </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-      <c r="D112">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
         <v>3</v>
       </c>
-      <c r="E112" s="79">
-        <v>1</v>
-      </c>
-      <c r="F112">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <v>2</v>
       </c>
-      <c r="G112">
+      <c r="G25">
         <v>114</v>
       </c>
-      <c r="H112">
-        <v>1</v>
-      </c>
-      <c r="I112">
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
         <v>288</v>
       </c>
-      <c r="J112">
+      <c r="J25">
         <v>934.33</v>
       </c>
-      <c r="K112">
+      <c r="K25">
         <v>70309.84</v>
       </c>
-      <c r="M112">
+      <c r="M25">
         <v>45663.32</v>
       </c>
-      <c r="P112">
+      <c r="P25">
         <v>7</v>
       </c>
-      <c r="Q112">
+      <c r="Q25">
         <v>0.54907976357843136</v>
       </c>
-      <c r="R112">
+      <c r="R25">
         <v>0.14268148165490191</v>
       </c>
     </row>
-    <row r="113" spans="1:18">
-      <c r="A113" t="s">
+    <row r="26" spans="1:18">
+      <c r="A26" t="s">
         <v>77</v>
       </c>
-      <c r="B113">
+      <c r="B26">
         <v>40</v>
       </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-      <c r="D113">
-        <v>1</v>
-      </c>
-      <c r="E113" s="79">
-        <v>1</v>
-      </c>
-      <c r="F113">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <v>2</v>
       </c>
-      <c r="G113">
+      <c r="G26">
         <v>115</v>
       </c>
-      <c r="H113">
-        <v>1</v>
-      </c>
-      <c r="I113">
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
         <v>288</v>
       </c>
-      <c r="J113">
+      <c r="J26">
         <v>934.33</v>
       </c>
-      <c r="K113">
+      <c r="K26">
         <v>179566.28</v>
       </c>
-      <c r="M113">
+      <c r="M26">
         <v>113900.89</v>
       </c>
-      <c r="P113">
+      <c r="P26">
         <v>7</v>
       </c>
-      <c r="Q113">
+      <c r="Q26">
         <v>1.4629057902083336</v>
       </c>
-      <c r="R113">
+      <c r="R26">
         <v>0.2625977758833335</v>
       </c>
     </row>
-    <row r="114" spans="1:18">
-      <c r="A114" t="s">
+    <row r="27" spans="1:18">
+      <c r="A27" t="s">
         <v>77</v>
       </c>
-      <c r="B114">
+      <c r="B27">
         <v>40</v>
       </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-      <c r="D114">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
         <v>2</v>
       </c>
-      <c r="E114" s="79">
-        <v>1</v>
-      </c>
-      <c r="F114">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
         <v>2</v>
       </c>
-      <c r="G114">
+      <c r="G27">
         <v>116</v>
       </c>
-      <c r="H114">
-        <v>1</v>
-      </c>
-      <c r="I114">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>288</v>
       </c>
-      <c r="J114">
+      <c r="J27">
         <v>934.33</v>
       </c>
-      <c r="K114">
+      <c r="K27">
         <v>171362.07</v>
       </c>
-      <c r="M114">
+      <c r="M27">
         <v>108815.26</v>
       </c>
-      <c r="P114">
+      <c r="P27">
         <v>7</v>
       </c>
-      <c r="Q114">
+      <c r="Q27">
         <v>1.3934294840563728</v>
       </c>
-      <c r="R114">
+      <c r="R27">
         <v>0.2550310255602935</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
-      <c r="A115" t="s">
+    <row r="28" spans="1:18">
+      <c r="A28" t="s">
         <v>77</v>
       </c>
-      <c r="B115">
+      <c r="B28">
         <v>40</v>
       </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
         <v>3</v>
       </c>
-      <c r="E115" s="79">
-        <v>1</v>
-      </c>
-      <c r="F115">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
         <v>2</v>
       </c>
-      <c r="G115">
+      <c r="G28">
         <v>117</v>
       </c>
-      <c r="H115">
-        <v>1</v>
-      </c>
-      <c r="I115">
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
         <v>288</v>
       </c>
-      <c r="J115">
+      <c r="J28">
         <v>934.33</v>
       </c>
-      <c r="K115">
+      <c r="K28">
         <v>180521.2</v>
       </c>
-      <c r="M115">
+      <c r="M28">
         <v>115821.34</v>
       </c>
-      <c r="P115">
+      <c r="P28">
         <v>7</v>
       </c>
-      <c r="Q115">
+      <c r="Q28">
         <v>1.4413955330147064</v>
       </c>
-      <c r="R115">
+      <c r="R28">
         <v>0.31320125020196005</v>
       </c>
     </row>
-    <row r="116" spans="1:18">
-      <c r="A116" t="s">
+    <row r="29" spans="1:18">
+      <c r="A29" t="s">
         <v>81</v>
       </c>
-      <c r="B116">
+      <c r="B29">
         <v>60</v>
       </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116">
-        <v>1</v>
-      </c>
-      <c r="E116" s="79">
-        <v>1</v>
-      </c>
-      <c r="F116">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>2</v>
       </c>
-      <c r="G116">
+      <c r="G29">
         <v>118</v>
       </c>
-      <c r="H116">
-        <v>1</v>
-      </c>
-      <c r="I116">
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>288</v>
       </c>
-      <c r="J116">
+      <c r="J29">
         <v>934.33</v>
       </c>
-      <c r="K116">
+      <c r="K29">
         <v>212295.54</v>
       </c>
-      <c r="M116">
+      <c r="M29">
         <v>136466.82</v>
       </c>
-      <c r="P116">
+      <c r="P29">
         <v>7</v>
       </c>
-      <c r="Q116">
+      <c r="Q29">
         <v>1.6893263491176471</v>
       </c>
-      <c r="R116">
+      <c r="R29">
         <v>0.37803225153235309</v>
       </c>
     </row>
-    <row r="117" spans="1:18">
-      <c r="A117" t="s">
+    <row r="30" spans="1:18">
+      <c r="A30" t="s">
         <v>81</v>
       </c>
-      <c r="B117">
+      <c r="B30">
         <v>60</v>
       </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-      <c r="D117">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="E117" s="79">
-        <v>1</v>
-      </c>
-      <c r="F117">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
         <v>2</v>
       </c>
-      <c r="G117">
+      <c r="G30">
         <v>119</v>
       </c>
-      <c r="H117">
-        <v>1</v>
-      </c>
-      <c r="I117">
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <v>288</v>
       </c>
-      <c r="J117">
+      <c r="J30">
         <v>934.33</v>
       </c>
-      <c r="K117">
+      <c r="K30">
         <v>201611.42</v>
       </c>
-      <c r="M117">
+      <c r="M30">
         <v>130322.87</v>
       </c>
-      <c r="P117">
+      <c r="P30">
         <v>7</v>
       </c>
-      <c r="Q117">
+      <c r="Q30">
         <v>1.5881795961397065</v>
       </c>
-      <c r="R117">
+      <c r="R30">
         <v>0.38610328196862664</v>
       </c>
     </row>
-    <row r="118" spans="1:18">
-      <c r="A118" t="s">
+    <row r="31" spans="1:18">
+      <c r="A31" t="s">
         <v>81</v>
       </c>
-      <c r="B118">
+      <c r="B31">
         <v>60</v>
       </c>
-      <c r="C118">
-        <v>1</v>
-      </c>
-      <c r="D118">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
         <v>3</v>
       </c>
-      <c r="E118" s="79">
-        <v>1</v>
-      </c>
-      <c r="F118">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>2</v>
       </c>
-      <c r="G118">
+      <c r="G31">
         <v>120</v>
       </c>
-      <c r="H118">
-        <v>1</v>
-      </c>
-      <c r="I118">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
         <v>288</v>
       </c>
-      <c r="J118">
+      <c r="J31">
         <v>934.33</v>
       </c>
-      <c r="K118">
+      <c r="K31">
         <v>214420.85</v>
       </c>
-      <c r="M118">
+      <c r="M31">
         <v>135199.67999999999</v>
       </c>
-      <c r="P118">
+      <c r="P31">
         <v>7</v>
       </c>
-      <c r="Q118">
+      <c r="Q31">
         <v>1.7649039821446082</v>
       </c>
-      <c r="R118">
+      <c r="R31">
         <v>0.28325850345539183</v>
       </c>
     </row>
-    <row r="119" spans="1:18">
-      <c r="A119" t="s">
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
         <v>86</v>
       </c>
-      <c r="B119">
+      <c r="B32">
         <v>80</v>
       </c>
-      <c r="C119">
-        <v>1</v>
-      </c>
-      <c r="D119">
-        <v>1</v>
-      </c>
-      <c r="E119" s="79">
-        <v>1</v>
-      </c>
-      <c r="F119">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <v>2</v>
       </c>
-      <c r="G119">
+      <c r="G32">
         <v>121</v>
       </c>
-      <c r="H119">
-        <v>1</v>
-      </c>
-      <c r="I119">
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>288</v>
       </c>
-      <c r="J119">
+      <c r="J32">
         <v>934.33</v>
       </c>
-      <c r="K119">
+      <c r="K32">
         <v>283023.03000000003</v>
       </c>
-      <c r="M119">
+      <c r="M32">
         <v>181904.32</v>
       </c>
-      <c r="P119">
+      <c r="P32">
         <v>7</v>
       </c>
-      <c r="Q119">
+      <c r="Q32">
         <v>2.2527414572181379</v>
       </c>
-      <c r="R119">
+      <c r="R32">
         <v>0.50295740384852916</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
-      <c r="A120" t="s">
+    <row r="33" spans="1:18">
+      <c r="A33" t="s">
         <v>86</v>
       </c>
-      <c r="B120">
+      <c r="B33">
         <v>80</v>
       </c>
-      <c r="C120">
-        <v>1</v>
-      </c>
-      <c r="D120">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
         <v>2</v>
       </c>
-      <c r="E120" s="79">
-        <v>1</v>
-      </c>
-      <c r="F120">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>2</v>
       </c>
-      <c r="G120">
+      <c r="G33">
         <v>122</v>
       </c>
-      <c r="H120">
-        <v>1</v>
-      </c>
-      <c r="I120">
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>288</v>
       </c>
-      <c r="J120">
+      <c r="J33">
         <v>934.33</v>
       </c>
-      <c r="K120">
+      <c r="K33">
         <v>284270.5</v>
       </c>
-      <c r="M120">
+      <c r="M33">
         <v>181308.84</v>
       </c>
-      <c r="P120">
+      <c r="P33">
         <v>7</v>
       </c>
-      <c r="Q120">
+      <c r="Q33">
         <v>2.2937990406127455</v>
       </c>
-      <c r="R120">
+      <c r="R33">
         <v>0.45287879468725445</v>
       </c>
     </row>
-    <row r="121" spans="1:18">
-      <c r="A121" t="s">
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
         <v>86</v>
       </c>
-      <c r="B121">
+      <c r="B34">
         <v>80</v>
       </c>
-      <c r="C121">
-        <v>1</v>
-      </c>
-      <c r="D121">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
         <v>3</v>
       </c>
-      <c r="E121" s="79">
-        <v>1</v>
-      </c>
-      <c r="F121">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>2</v>
       </c>
-      <c r="G121">
+      <c r="G34">
         <v>123</v>
       </c>
-      <c r="H121">
-        <v>1</v>
-      </c>
-      <c r="I121">
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
         <v>288</v>
       </c>
-      <c r="J121">
+      <c r="J34">
         <v>934.33</v>
       </c>
-      <c r="K121">
+      <c r="K34">
         <v>285379.81</v>
       </c>
-      <c r="M121">
+      <c r="M34">
         <v>190202.59</v>
       </c>
-      <c r="P121">
+      <c r="P34">
         <v>7</v>
       </c>
-      <c r="Q121">
+      <c r="Q34">
         <v>2.1203758362500005</v>
       </c>
-      <c r="R121">
+      <c r="R34">
         <v>0.7610349000916663</v>
       </c>
     </row>
-    <row r="122" spans="1:18">
-      <c r="A122" t="s">
+    <row r="35" spans="1:18">
+      <c r="A35" t="s">
         <v>88</v>
       </c>
-      <c r="B122">
+      <c r="B35">
         <v>100</v>
       </c>
-      <c r="C122">
-        <v>1</v>
-      </c>
-      <c r="D122">
-        <v>1</v>
-      </c>
-      <c r="E122" s="79">
-        <v>1</v>
-      </c>
-      <c r="F122">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>2</v>
       </c>
-      <c r="G122">
+      <c r="G35">
         <v>124</v>
       </c>
-      <c r="H122">
-        <v>1</v>
-      </c>
-      <c r="I122">
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <v>288</v>
       </c>
-      <c r="J122">
+      <c r="J35">
         <v>934.33</v>
       </c>
-      <c r="K122">
+      <c r="K35">
         <v>348560.28</v>
       </c>
-      <c r="M122">
+      <c r="M35">
         <v>244957.82</v>
       </c>
-      <c r="P122">
+      <c r="P35">
         <v>7</v>
       </c>
-      <c r="Q122">
+      <c r="Q35">
         <v>2.3080749023774518</v>
       </c>
-      <c r="R122">
+      <c r="R35">
         <v>1.4028319391058823</v>
       </c>
     </row>
-    <row r="123" spans="1:18">
-      <c r="A123" t="s">
+    <row r="36" spans="1:18">
+      <c r="A36" t="s">
         <v>88</v>
       </c>
-      <c r="B123">
+      <c r="B36">
         <v>100</v>
       </c>
-      <c r="C123">
-        <v>1</v>
-      </c>
-      <c r="D123">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
         <v>2</v>
       </c>
-      <c r="E123" s="79">
-        <v>1</v>
-      </c>
-      <c r="F123">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>2</v>
       </c>
-      <c r="G123">
+      <c r="G36">
         <v>125</v>
       </c>
-      <c r="H123">
-        <v>1</v>
-      </c>
-      <c r="I123">
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
         <v>288</v>
       </c>
-      <c r="J123">
+      <c r="J36">
         <v>934.33</v>
       </c>
-      <c r="K123">
+      <c r="K36">
         <v>362923.71</v>
       </c>
-      <c r="M123">
+      <c r="M36">
         <v>234319.96</v>
       </c>
-      <c r="P123">
+      <c r="P36">
         <v>7</v>
       </c>
-      <c r="Q123">
+      <c r="Q36">
         <v>2.8650582981004908</v>
       </c>
-      <c r="R123">
+      <c r="R36">
         <v>0.68469382926617584</v>
       </c>
     </row>
-    <row r="124" spans="1:18">
-      <c r="A124" t="s">
+    <row r="37" spans="1:18">
+      <c r="A37" t="s">
         <v>88</v>
       </c>
-      <c r="B124">
+      <c r="B37">
         <v>100</v>
       </c>
-      <c r="C124">
-        <v>1</v>
-      </c>
-      <c r="D124">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
         <v>3</v>
       </c>
-      <c r="E124" s="79">
-        <v>1</v>
-      </c>
-      <c r="F124">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>2</v>
       </c>
-      <c r="G124">
+      <c r="G37">
         <v>126</v>
       </c>
-      <c r="H124">
-        <v>1</v>
-      </c>
-      <c r="I124">
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
         <v>288</v>
       </c>
-      <c r="J124">
+      <c r="J37">
         <v>934.33</v>
       </c>
-      <c r="K124">
+      <c r="K37">
         <v>413253.5</v>
       </c>
-      <c r="M124">
+      <c r="M37">
         <v>264688.12</v>
       </c>
-      <c r="P124">
+      <c r="P37">
         <v>7</v>
       </c>
-      <c r="Q124">
+      <c r="Q37">
         <v>3.3097672095833337</v>
       </c>
-      <c r="R124">
+      <c r="R37">
         <v>0.70003723498333337</v>
       </c>
     </row>
-    <row r="125" spans="1:18">
-      <c r="A125" t="s">
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
         <v>90</v>
       </c>
-      <c r="B125">
+      <c r="B38">
         <v>100</v>
       </c>
-      <c r="C125">
+      <c r="C38">
         <v>0</v>
       </c>
-      <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="E125" s="79">
-        <v>1</v>
-      </c>
-      <c r="F125">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
         <v>2</v>
       </c>
-      <c r="G125">
+      <c r="G38">
         <v>127</v>
       </c>
-      <c r="H125">
-        <v>1</v>
-      </c>
-      <c r="I125">
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
         <v>288</v>
       </c>
-      <c r="J125">
+      <c r="J38">
         <v>934.33</v>
       </c>
-      <c r="K125">
+      <c r="K38">
         <v>314445.78000000003</v>
       </c>
-      <c r="M125">
+      <c r="M38">
         <v>201123.25</v>
       </c>
-      <c r="P125">
+      <c r="P38">
         <v>7</v>
       </c>
-      <c r="Q125">
+      <c r="Q38">
         <v>2.5246204324387262</v>
       </c>
-      <c r="R125">
+      <c r="R38">
         <v>0.52222920235294057</v>
       </c>
     </row>
-    <row r="126" spans="1:18">
-      <c r="A126" t="s">
+    <row r="39" spans="1:18">
+      <c r="A39" t="s">
         <v>90</v>
       </c>
-      <c r="B126">
+      <c r="B39">
         <v>100</v>
       </c>
-      <c r="C126">
+      <c r="C39">
         <v>0</v>
       </c>
-      <c r="D126">
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="E126" s="79">
-        <v>1</v>
-      </c>
-      <c r="F126">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <v>2</v>
       </c>
-      <c r="G126">
+      <c r="G39">
         <v>128</v>
       </c>
-      <c r="H126">
-        <v>1</v>
-      </c>
-      <c r="I126">
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <v>288</v>
       </c>
-      <c r="J126">
+      <c r="J39">
         <v>934.33</v>
       </c>
-      <c r="K126">
+      <c r="K39">
         <v>319769.46000000002</v>
       </c>
-      <c r="M126">
+      <c r="M39">
         <v>201787.5</v>
       </c>
-      <c r="P126">
+      <c r="P39">
         <v>7</v>
       </c>
-      <c r="Q126">
+      <c r="Q39">
         <v>2.6284240819117652</v>
       </c>
-      <c r="R126">
+      <c r="R39">
         <v>0.42848838683823492</v>
       </c>
     </row>
-    <row r="127" spans="1:18">
-      <c r="A127" t="s">
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
         <v>90</v>
       </c>
-      <c r="B127">
+      <c r="B40">
         <v>100</v>
       </c>
-      <c r="C127">
+      <c r="C40">
         <v>0</v>
       </c>
-      <c r="D127">
+      <c r="D40">
         <v>3</v>
       </c>
-      <c r="E127" s="79">
-        <v>1</v>
-      </c>
-      <c r="F127">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <v>2</v>
       </c>
-      <c r="G127">
+      <c r="G40">
         <v>129</v>
       </c>
-      <c r="H127">
-        <v>1</v>
-      </c>
-      <c r="I127">
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
         <v>288</v>
       </c>
-      <c r="J127">
+      <c r="J40">
         <v>934.33</v>
       </c>
-      <c r="K127">
+      <c r="K40">
         <v>383054.37</v>
       </c>
-      <c r="M127">
+      <c r="M40">
         <v>242358.89</v>
       </c>
-      <c r="P127">
+      <c r="P40">
         <v>7</v>
       </c>
-      <c r="Q127">
+      <c r="Q40">
         <v>3.1344401114215685</v>
       </c>
-      <c r="R127">
+      <c r="R40">
         <v>0.53709510633676516</v>
       </c>
     </row>
-    <row r="128" spans="1:18">
-      <c r="A128" t="s">
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
         <v>169</v>
       </c>
-      <c r="B128">
+      <c r="B41">
         <v>20</v>
       </c>
-      <c r="C128">
+      <c r="C41">
         <v>0</v>
       </c>
-      <c r="D128">
-        <v>1</v>
-      </c>
-      <c r="E128" s="79">
-        <v>1</v>
-      </c>
-      <c r="F128">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>2</v>
       </c>
-      <c r="G128">
+      <c r="G41">
         <v>130</v>
       </c>
-      <c r="H128">
-        <v>1</v>
-      </c>
-      <c r="I128">
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
         <v>288</v>
       </c>
-      <c r="J128">
+      <c r="J41">
         <v>934.33</v>
       </c>
-      <c r="K128">
+      <c r="K41">
         <v>62118.78</v>
       </c>
-      <c r="M128">
+      <c r="M41">
         <v>40189.17</v>
       </c>
-      <c r="P128">
+      <c r="P41">
         <v>7</v>
       </c>
-      <c r="Q128">
+      <c r="Q41">
         <v>0.48855193650735296</v>
       </c>
-      <c r="R128">
+      <c r="R41">
         <v>0.12028049801764694</v>
       </c>
     </row>
-    <row r="129" spans="1:18">
-      <c r="A129" t="s">
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
         <v>169</v>
       </c>
-      <c r="B129">
+      <c r="B42">
         <v>20</v>
       </c>
-      <c r="C129">
+      <c r="C42">
         <v>0</v>
       </c>
-      <c r="D129">
+      <c r="D42">
         <v>2</v>
       </c>
-      <c r="E129" s="79">
-        <v>1</v>
-      </c>
-      <c r="F129">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <v>2</v>
       </c>
-      <c r="G129">
+      <c r="G42">
         <v>131</v>
       </c>
-      <c r="H129">
-        <v>1</v>
-      </c>
-      <c r="I129">
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
         <v>288</v>
       </c>
-      <c r="J129">
+      <c r="J42">
         <v>934.33</v>
       </c>
-      <c r="K129">
+      <c r="K42">
         <v>78061.3</v>
       </c>
-      <c r="M129">
+      <c r="M42">
         <v>49939.89</v>
       </c>
-      <c r="P129">
+      <c r="P42">
         <v>7</v>
       </c>
-      <c r="Q129">
+      <c r="Q42">
         <v>0.62649401028186291</v>
       </c>
-      <c r="R129">
+      <c r="R42">
         <v>0.13005370664313709</v>
       </c>
     </row>
-    <row r="130" spans="1:18">
-      <c r="A130" t="s">
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
         <v>169</v>
       </c>
-      <c r="B130">
+      <c r="B43">
         <v>20</v>
       </c>
-      <c r="C130">
+      <c r="C43">
         <v>0</v>
       </c>
-      <c r="D130">
+      <c r="D43">
         <v>3</v>
       </c>
-      <c r="E130" s="79">
-        <v>1</v>
-      </c>
-      <c r="F130">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>2</v>
       </c>
-      <c r="G130">
+      <c r="G43">
         <v>132</v>
       </c>
-      <c r="H130">
-        <v>1</v>
-      </c>
-      <c r="I130">
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
         <v>288</v>
       </c>
-      <c r="J130">
+      <c r="J43">
         <v>934.33</v>
       </c>
-      <c r="K130">
+      <c r="K43">
         <v>101733.5</v>
       </c>
-      <c r="M130">
+      <c r="M43">
         <v>65084.160000000003</v>
       </c>
-      <c r="O130">
+      <c r="O43">
         <v>905.76</v>
       </c>
-      <c r="P130">
+      <c r="P43">
         <v>7</v>
       </c>
-      <c r="Q130">
+      <c r="Q43">
         <v>0.81648082335784311</v>
       </c>
-      <c r="R130">
+      <c r="R43">
         <v>0.16948996384215689</v>
       </c>
     </row>

</xml_diff>